<commit_message>
Updated testing documentation and app configuration after the first three reference page tests
</commit_message>
<xml_diff>
--- a/CRDMA/docs/Cruise Data Management Application - Reference Preset Page Inventory.xlsx
+++ b/CRDMA/docs/Cruise Data Management Application - Reference Preset Page Inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Lists" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Page Name</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Data Set Status</t>
+  </si>
+  <si>
+    <t>Data Set Type</t>
   </si>
 </sst>
 </file>
@@ -117,9 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,19 +407,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,124 +427,98 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B2" s="2">
+        <v>45264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>17</v>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45264</v>
       </c>
     </row>
   </sheetData>
@@ -550,17 +531,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -576,7 +557,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -584,7 +565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -592,7 +573,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -600,7 +581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -608,7 +589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -616,7 +597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -624,7 +605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
DB data model bug fix
</commit_message>
<xml_diff>
--- a/CRDMA/docs/Cruise Data Management Application - Reference Preset Page Inventory.xlsx
+++ b/CRDMA/docs/Cruise Data Management Application - Reference Preset Page Inventory.xlsx
@@ -410,7 +410,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A11" sqref="A11:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,40 +439,64 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="2">
+        <v>45265</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="2">
+        <v>45265</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="2">
+        <v>45265</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="2">
+        <v>45265</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="2">
+        <v>45265</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="2">
+        <v>45265</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" s="2">
+        <v>45265</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45265</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding the CCM DB upgrade and implemented/documented the DLM configuration
</commit_message>
<xml_diff>
--- a/CRDMA/docs/Cruise Data Management Application - Reference Preset Page Inventory.xlsx
+++ b/CRDMA/docs/Cruise Data Management Application - Reference Preset Page Inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Lists" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Page Name</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Testing Completed?</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>Data Set Status</t>
@@ -409,7 +406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +546,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <v>45264</v>
@@ -557,7 +554,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2">
         <v>45264</v>
@@ -573,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,64 +592,40 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>